<commit_message>
pract reactby ranmansir react router dom
</commit_message>
<xml_diff>
--- a/leetcode/SepNeetcodeSakshi(AutoRecovered).xlsx
+++ b/leetcode/SepNeetcodeSakshi(AutoRecovered).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakshisrivastava/Desktop/hanumant_fullstack/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D7E61E-9136-B54F-AAF4-E97B964CBCD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34EAF764-3A83-2A4D-9BF9-A4CC9F778759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15560" xr2:uid="{7223D205-73F4-4148-BF4C-16C1EFE483E0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
   <si>
     <t>Sakshi neetcode Track</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>graph start</t>
+  </si>
+  <si>
+    <t>25. dyas</t>
   </si>
 </sst>
 </file>
@@ -715,7 +718,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -969,7 +972,15 @@
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
+      <c r="G12" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="13">
+        <v>73</v>
+      </c>
+      <c r="M12" t="s">
+        <v>54</v>
+      </c>
       <c r="N12" t="s">
         <v>53</v>
       </c>

</xml_diff>